<commit_message>
Funcionalidades Listas para Entrega
</commit_message>
<xml_diff>
--- a/data/inventario.xlsx
+++ b/data/inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,287 +436,346 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>producto</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>cantidad</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>ultima_actualizacion</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Tomate</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>200</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>187</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>2025-06-18</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Cebolla</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>113</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>2025-06-25</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Carne de cerdo</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-06-17</t>
+      <c r="C4" t="n">
+        <v>114</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Naranja</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>244</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>2025-06-25</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Papa</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>180</v>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>184</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>2025-06-20</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Banano</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>68</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>98</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>2025-06-25</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Zanahoria</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>160</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>154</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>2025-06-22</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Leche</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>100</v>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>96</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>2025-06-15</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Pera</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>140</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>2025-06-14</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Manzana</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>120</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2025-06-13</t>
+      <c r="C11" t="n">
+        <v>140</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Habichuela</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>160</v>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>159</v>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>2025-06-18</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Carne de res</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>53</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2025-06-19</t>
+      <c r="C13" t="n">
+        <v>109</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Uvas</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>120</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2025-06-17</t>
+      <c r="C14" t="n">
+        <v>128</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Papaya</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>42</v>
-      </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="n">
+        <v>85</v>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>2025-06-25</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Mango</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>100</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>2025-06-20</t>
+      <c r="C16" t="n">
+        <v>101</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Auyama</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>60</v>
-      </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" t="n">
+        <v>84</v>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>2025-06-21</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Pollo</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>60</v>
-      </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="n">
+        <v>92</v>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>2025-06-22</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Apio</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>38</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2025-06-25</t>
+      <c r="C19" t="n">
+        <v>80</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
         </is>
       </c>
     </row>

</xml_diff>